<commit_message>
burden factor / divergence factor
</commit_message>
<xml_diff>
--- a/bytype.xlsx
+++ b/bytype.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="bytype" sheetId="1" r:id="rId1"/>
@@ -763,11 +763,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1089,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,7 +1108,7 @@
     <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>73</v>
       </c>
@@ -1140,7 +1141,7 @@
         <v>4.7275626466517826</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>72</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>6.1521838599659855</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -1234,41 +1235,49 @@
         <f t="shared" ref="J4:J35" si="2">G4/I4</f>
         <v>5.5641025641025639</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <f>H4/$H$2</f>
+        <v>6.9526664965552429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>109</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>23131</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>212</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>3900</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>35</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>1461</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>13</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <f t="shared" si="2"/>
         <v>2.6923076923076925</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="4">
+        <f t="shared" ref="K5:K19" si="3">H5/$H$2</f>
+        <v>11.743174279152845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>49</v>
       </c>
@@ -1300,8 +1309,12 @@
         <f t="shared" si="2"/>
         <v>13.211538461538462</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>1.6798928298035212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>38</v>
       </c>
@@ -1333,8 +1346,12 @@
         <f t="shared" si="2"/>
         <v>15.65625</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>1.3021178872161265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>17</v>
       </c>
@@ -1366,8 +1383,12 @@
         <f t="shared" si="2"/>
         <v>18.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>1.028833886195458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>39</v>
       </c>
@@ -1399,8 +1420,12 @@
         <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>3.1668793059453941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
@@ -1432,8 +1457,12 @@
         <f t="shared" si="2"/>
         <v>10.617647058823529</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>1.3664200051033426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>18</v>
       </c>
@@ -1465,8 +1494,12 @@
         <f t="shared" si="2"/>
         <v>9.3333333333333339</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>1.567364123500893</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>45</v>
       </c>
@@ -1498,8 +1531,12 @@
         <f t="shared" si="2"/>
         <v>4.6521739130434785</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>2.8132176575657053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1531,8 +1568,12 @@
         <f t="shared" si="2"/>
         <v>7.71875</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>1.551288594029089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1564,8 +1605,12 @@
         <f t="shared" si="2"/>
         <v>7.870967741935484</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>1.495024240877775</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1597,8 +1642,12 @@
         <f t="shared" si="2"/>
         <v>13.181818181818182</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>0.81181423832610355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1630,8 +1679,12 @@
         <f t="shared" si="2"/>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>3.600918601684103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>37</v>
       </c>
@@ -1663,8 +1716,12 @@
         <f t="shared" si="2"/>
         <v>13.025</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>0.64302117887216126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1696,8 +1753,12 @@
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>2.017478948711406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1729,8 +1790,12 @@
         <f t="shared" si="2"/>
         <v>5.5263157894736841</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>1.2699668282725185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>51</v>
       </c>
@@ -1763,7 +1828,7 @@
         <v>2.5909090909090908</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>35</v>
       </c>
@@ -1796,7 +1861,7 @@
         <v>8.6052631578947363</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>41</v>
       </c>
@@ -1829,7 +1894,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>42</v>
       </c>
@@ -1862,7 +1927,7 @@
         <v>5.9523809523809526</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>30</v>
       </c>
@@ -1895,7 +1960,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1928,7 +1993,7 @@
         <v>4.5714285714285712</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>40</v>
       </c>
@@ -1961,7 +2026,7 @@
         <v>3.6363636363636362</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1994,7 +2059,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8</v>
       </c>
@@ -2027,7 +2092,7 @@
         <v>5.6363636363636367</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>47</v>
       </c>
@@ -2060,7 +2125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2093,7 +2158,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20</v>
       </c>
@@ -2126,7 +2191,7 @@
         <v>3.0909090909090908</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2287,7 +2352,7 @@
         <v>9</v>
       </c>
       <c r="J36">
-        <f t="shared" ref="J36:J67" si="3">G36/I36</f>
+        <f t="shared" ref="J36:J66" si="4">G36/I36</f>
         <v>2.6666666666666665</v>
       </c>
     </row>
@@ -2320,7 +2385,7 @@
         <v>10</v>
       </c>
       <c r="J37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.6</v>
       </c>
     </row>
@@ -2353,7 +2418,7 @@
         <v>13</v>
       </c>
       <c r="J38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.615384615384615</v>
       </c>
     </row>
@@ -2386,7 +2451,7 @@
         <v>15</v>
       </c>
       <c r="J39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.3333333333333339</v>
       </c>
     </row>
@@ -2419,7 +2484,7 @@
         <v>5</v>
       </c>
       <c r="J40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4</v>
       </c>
     </row>
@@ -2452,7 +2517,7 @@
         <v>18</v>
       </c>
       <c r="J41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
     </row>
@@ -2485,7 +2550,7 @@
         <v>11</v>
       </c>
       <c r="J42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9090909090909092</v>
       </c>
     </row>
@@ -2518,7 +2583,7 @@
         <v>10</v>
       </c>
       <c r="J43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2551,7 +2616,7 @@
         <v>4</v>
       </c>
       <c r="J44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
     </row>
@@ -2584,7 +2649,7 @@
         <v>11</v>
       </c>
       <c r="J45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.72727272727272729</v>
       </c>
     </row>
@@ -2617,7 +2682,7 @@
         <v>5</v>
       </c>
       <c r="J46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.6</v>
       </c>
     </row>
@@ -2650,7 +2715,7 @@
         <v>34</v>
       </c>
       <c r="J47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6470588235294117</v>
       </c>
     </row>
@@ -2683,7 +2748,7 @@
         <v>20</v>
       </c>
       <c r="J48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2716,7 +2781,7 @@
         <v>18</v>
       </c>
       <c r="J49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
     </row>
@@ -2749,7 +2814,7 @@
         <v>10</v>
       </c>
       <c r="J50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.4</v>
       </c>
     </row>
@@ -2782,7 +2847,7 @@
         <v>9</v>
       </c>
       <c r="J51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4444444444444446</v>
       </c>
     </row>
@@ -2815,7 +2880,7 @@
         <v>7</v>
       </c>
       <c r="J52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4285714285714288</v>
       </c>
     </row>
@@ -2848,7 +2913,7 @@
         <v>2</v>
       </c>
       <c r="J53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.5</v>
       </c>
     </row>
@@ -2881,7 +2946,7 @@
         <v>7</v>
       </c>
       <c r="J54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.7142857142857144</v>
       </c>
     </row>
@@ -2914,7 +2979,7 @@
         <v>7</v>
       </c>
       <c r="J55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.8571428571428568</v>
       </c>
     </row>
@@ -2947,7 +3012,7 @@
         <v>13</v>
       </c>
       <c r="J56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8461538461538463</v>
       </c>
     </row>
@@ -2980,7 +3045,7 @@
         <v>8</v>
       </c>
       <c r="J57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.5</v>
       </c>
     </row>
@@ -3013,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="J58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3046,7 +3111,7 @@
         <v>9</v>
       </c>
       <c r="J59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
     </row>
@@ -3079,7 +3144,7 @@
         <v>7</v>
       </c>
       <c r="J60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.7142857142857142</v>
       </c>
     </row>
@@ -3112,7 +3177,7 @@
         <v>4</v>
       </c>
       <c r="J61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3145,7 +3210,7 @@
         <v>3</v>
       </c>
       <c r="J62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3178,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="J63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
@@ -3211,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="J64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -3244,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="J65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3277,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="J66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3294,7 +3359,7 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5905,31 +5970,31 @@
         <v>73</v>
       </c>
       <c r="M1">
-        <f>_xlfn.STDEV.P(D4:D66)</f>
+        <f t="shared" ref="M1:S1" si="0">_xlfn.STDEV.P(D4:D66)</f>
         <v>1.5822095818510133</v>
       </c>
       <c r="N1">
-        <f>_xlfn.STDEV.P(E4:E66)</f>
+        <f t="shared" si="0"/>
         <v>0.9197793986088002</v>
       </c>
       <c r="O1">
-        <f>_xlfn.STDEV.P(F4:F66)</f>
+        <f t="shared" si="0"/>
         <v>1.4870412472563208</v>
       </c>
       <c r="P1">
-        <f>_xlfn.STDEV.P(G4:G66)</f>
+        <f t="shared" si="0"/>
         <v>1.2975305914100748</v>
       </c>
       <c r="Q1">
-        <f>_xlfn.STDEV.P(H4:H66)</f>
+        <f t="shared" si="0"/>
         <v>1.7658648565515955</v>
       </c>
       <c r="R1">
-        <f>_xlfn.STDEV.P(I4:I66)</f>
+        <f t="shared" si="0"/>
         <v>0.87906266530066279</v>
       </c>
       <c r="S1">
-        <f>_xlfn.STDEV.P(J4:J66)</f>
+        <f t="shared" si="0"/>
         <v>0.76231340466748987</v>
       </c>
     </row>
@@ -5943,27 +6008,27 @@
         <v>62.999999999999986</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:J2" si="0">SUM(E4:E66)</f>
+        <f t="shared" ref="E2:J2" si="1">SUM(E4:E66)</f>
         <v>63.000000000000014</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.000000000000007</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.000000000000007</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.999999999999993</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.000000000000007</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.999999999999979</v>
       </c>
       <c r="K2" s="1">
@@ -5974,31 +6039,31 @@
         <v>72</v>
       </c>
       <c r="M2" s="1">
-        <f>AVERAGE(D4:D66)</f>
+        <f t="shared" ref="M2:S2" si="2">AVERAGE(D4:D66)</f>
         <v>0.99999999999999978</v>
       </c>
       <c r="N2" s="1">
-        <f>AVERAGE(E4:E66)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="O2" s="1">
-        <f>AVERAGE(F4:F66)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="P2" s="1">
-        <f>AVERAGE(G4:G66)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="Q2" s="1">
-        <f>AVERAGE(H4:H66)</f>
+        <f t="shared" si="2"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="R2" s="1">
-        <f>AVERAGE(I4:I66)</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="S2" s="1">
-        <f>AVERAGE(J4:J66)</f>
+        <f t="shared" si="2"/>
         <v>0.99999999999999967</v>
       </c>
       <c r="T2" s="1">
@@ -6100,39 +6165,39 @@
         <v>2.1474550764826308</v>
       </c>
       <c r="K4" s="1">
-        <f>(F4/$F$2)/(C4/$C$2)</f>
+        <f t="shared" ref="K4:K35" si="3">(F4/$F$2)/(C4/$C$2)</f>
         <v>9.7939170825715252</v>
       </c>
       <c r="M4">
-        <f>(D4-$M$2)/$M$1</f>
+        <f t="shared" ref="M4:M35" si="4">(D4-$M$2)/$M$1</f>
         <v>0.40514305135315126</v>
       </c>
       <c r="N4">
-        <f>(E4-$N$2)/$N$1</f>
+        <f t="shared" ref="N4:N35" si="5">(E4-$N$2)/$N$1</f>
         <v>2.1614089067159132</v>
       </c>
       <c r="O4">
-        <f>(F4-$O$2)/$O$1</f>
+        <f t="shared" ref="O4:O35" si="6">(F4-$O$2)/$O$1</f>
         <v>2.2039823481872247</v>
       </c>
       <c r="P4">
-        <f>(G4-$P$2)/$P$1</f>
+        <f t="shared" ref="P4:P35" si="7">(G4-$P$2)/$P$1</f>
         <v>3.707280691942596</v>
       </c>
       <c r="Q4">
-        <f>(H4-$Q$2)/$Q$1</f>
+        <f t="shared" ref="Q4:Q35" si="8">(H4-$Q$2)/$Q$1</f>
         <v>0.38501974105267889</v>
       </c>
       <c r="R4">
-        <f>(I4-$R$2)/$R$1</f>
+        <f t="shared" ref="R4:R35" si="9">(I4-$R$2)/$R$1</f>
         <v>2.5705806670386062</v>
       </c>
       <c r="S4">
-        <f>(J4-$S$2)/$S$1</f>
+        <f t="shared" ref="S4:S35" si="10">(J4-$S$2)/$S$1</f>
         <v>1.5052274687248017</v>
       </c>
       <c r="T4">
-        <f>ABS(M4)+ABS(N4)+ABS(O4)+ABS(P4)+ABS(Q4)+ABS(R4)+ABS(S4)</f>
+        <f t="shared" ref="T4:T35" si="11">ABS(M4)+ABS(N4)+ABS(O4)+ABS(P4)+ABS(Q4)+ABS(R4)+ABS(S4)</f>
         <v>12.93864287501497</v>
       </c>
       <c r="U4" t="s">
@@ -6174,39 +6239,39 @@
         <v>2.1171343861742153</v>
       </c>
       <c r="K5" s="1">
-        <f>(F5/$F$2)/(C5/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>7.4274101892572997</v>
       </c>
       <c r="M5">
-        <f>(D5-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.241248731668914</v>
       </c>
       <c r="N5">
-        <f>(E5-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.3592410553869485</v>
       </c>
       <c r="O5">
-        <f>(F5-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.41823327303858876</v>
       </c>
       <c r="P5">
-        <f>(G5-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>2.6252662502051645</v>
       </c>
       <c r="Q5">
-        <f>(H5-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.20215523277639244</v>
       </c>
       <c r="R5">
-        <f>(I5-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.7148523604418711</v>
       </c>
       <c r="S5">
-        <f>(J5-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>1.4654528955338175</v>
       </c>
       <c r="T5">
-        <f>ABS(M5)+ABS(N5)+ABS(O5)+ABS(P5)+ABS(Q5)+ABS(R5)+ABS(S5)</f>
+        <f t="shared" si="11"/>
         <v>8.0264497990516954</v>
       </c>
       <c r="U5" t="s">
@@ -6248,39 +6313,39 @@
         <v>2.5448280409627682</v>
       </c>
       <c r="K6" s="1">
-        <f>(F6/$F$2)/(C6/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>7.1422888768098023</v>
       </c>
       <c r="M6">
-        <f>(D6-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.443902027337017</v>
       </c>
       <c r="N6">
-        <f>(E6-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.6081896989028344</v>
       </c>
       <c r="O6">
-        <f>(F6-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.9496230133331109</v>
       </c>
       <c r="P6">
-        <f>(G6-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>2.4949030644536663</v>
       </c>
       <c r="Q6">
-        <f>(H6-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.17108777384363744</v>
       </c>
       <c r="R6">
-        <f>(I6-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.1443668227107135</v>
       </c>
       <c r="S6">
-        <f>(J6-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>2.0264999034571618</v>
       </c>
       <c r="T6">
-        <f>ABS(M6)+ABS(N6)+ABS(O6)+ABS(P6)+ABS(Q6)+ABS(R6)+ABS(S6)</f>
+        <f t="shared" si="11"/>
         <v>9.8385723040381414</v>
       </c>
       <c r="U6" t="s">
@@ -6322,39 +6387,39 @@
         <v>2.9582991039056208</v>
       </c>
       <c r="K7" s="1">
-        <f>(F7/$F$2)/(C7/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>6.4922122844295096</v>
       </c>
       <c r="M7">
-        <f>(D7-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.34038121806365396</v>
       </c>
       <c r="N7">
-        <f>(E7-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.3469472952133246</v>
       </c>
       <c r="O7">
-        <f>(F7-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.7109648719885098</v>
       </c>
       <c r="P7">
-        <f>(G7-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>2.1950677372252207</v>
       </c>
       <c r="Q7">
-        <f>(H7-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>1.6328478415820181E-2</v>
       </c>
       <c r="R7">
-        <f>(I7-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.64519197719595134</v>
       </c>
       <c r="S7">
-        <f>(J7-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>2.5688897662239105</v>
       </c>
       <c r="T7">
-        <f>ABS(M7)+ABS(N7)+ABS(O7)+ABS(P7)+ABS(Q7)+ABS(R7)+ABS(S7)</f>
+        <f t="shared" si="11"/>
         <v>8.8237713443263921</v>
       </c>
       <c r="U7" t="s">
@@ -6396,39 +6461,39 @@
         <v>2.14262422610547</v>
       </c>
       <c r="K8" s="1">
-        <f>(F8/$F$2)/(C8/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>6.2061405676071866</v>
       </c>
       <c r="M8">
-        <f>(D8-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.16792830593290953</v>
       </c>
       <c r="N8">
-        <f>(E8-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>2.2536121080180926</v>
       </c>
       <c r="O8">
-        <f>(F8-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.69457427880602129</v>
       </c>
       <c r="P8">
-        <f>(G8-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>2.064704551473723</v>
       </c>
       <c r="Q8">
-        <f>(H8-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.10656860912979943</v>
       </c>
       <c r="R8">
-        <f>(I8-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.2156775149271086</v>
       </c>
       <c r="S8">
-        <f>(J8-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>1.4988903764638202</v>
       </c>
       <c r="T8">
-        <f>ABS(M8)+ABS(N8)+ABS(O8)+ABS(P8)+ABS(Q8)+ABS(R8)+ABS(S8)</f>
+        <f t="shared" si="11"/>
         <v>8.0019557447514735</v>
       </c>
       <c r="U8" t="s">
@@ -6470,39 +6535,39 @@
         <v>0.90441096864964743</v>
       </c>
       <c r="K9" s="1">
-        <f>(F9/$F$2)/(C9/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>6.1871324801106882</v>
       </c>
       <c r="M9">
-        <f>(D9-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>3.877260431578696</v>
       </c>
       <c r="N9">
-        <f>(E9-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>4.048501093367193</v>
       </c>
       <c r="O9">
-        <f>(F9-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>4.3246902182054763</v>
       </c>
       <c r="P9">
-        <f>(G9-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>2.0581863921861481</v>
       </c>
       <c r="Q9">
-        <f>(H9-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>3.3709637940129178</v>
       </c>
       <c r="R9">
-        <f>(I9-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>4.4246586646648671</v>
       </c>
       <c r="S9">
-        <f>(J9-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.12539334972346025</v>
       </c>
       <c r="T9">
-        <f>ABS(M9)+ABS(N9)+ABS(O9)+ABS(P9)+ABS(Q9)+ABS(R9)+ABS(S9)</f>
+        <f t="shared" si="11"/>
         <v>22.229653943738761</v>
       </c>
       <c r="U9" t="s">
@@ -6544,39 +6609,39 @@
         <v>1.7258338340496593</v>
       </c>
       <c r="K10" s="1">
-        <f>(F10/$F$2)/(C10/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>5.1578445421752219</v>
       </c>
       <c r="M10">
-        <f>(D10-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.35092954697065548</v>
       </c>
       <c r="N10">
-        <f>(E10-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.3746082556039789</v>
       </c>
       <c r="O10">
-        <f>(F10-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.2210876344916977</v>
       </c>
       <c r="P10">
-        <f>(G10-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>1.5823607641931812</v>
       </c>
       <c r="Q10">
-        <f>(H10-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.20750172570900619</v>
       </c>
       <c r="R10">
-        <f>(I10-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.286988207143503</v>
       </c>
       <c r="S10">
-        <f>(J10-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.95214622962882034</v>
       </c>
       <c r="T10">
-        <f>ABS(M10)+ABS(N10)+ABS(O10)+ABS(P10)+ABS(Q10)+ABS(R10)+ABS(S10)</f>
+        <f t="shared" si="11"/>
         <v>6.9756223637408432</v>
       </c>
       <c r="U10" t="s">
@@ -6618,39 +6683,39 @@
         <v>3.1696061827560227</v>
       </c>
       <c r="K11" s="1">
-        <f>(F11/$F$2)/(C11/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>5.0038790334535745</v>
       </c>
       <c r="M11">
-        <f>(D11-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.50888191393725302</v>
       </c>
       <c r="N11">
-        <f>(E11-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>0.45564968262558664</v>
       </c>
       <c r="O11">
-        <f>(F11-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.30506837463298653</v>
       </c>
       <c r="P11">
-        <f>(G11-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>1.5171791713174319</v>
       </c>
       <c r="Q11">
-        <f>(H11-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.48436335973300038</v>
       </c>
       <c r="R11">
-        <f>(I11-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.14601713168118866</v>
       </c>
       <c r="S11">
-        <f>(J11-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>2.8460816371219053</v>
       </c>
       <c r="T11">
-        <f>ABS(M11)+ABS(N11)+ABS(O11)+ABS(P11)+ABS(Q11)+ABS(R11)+ABS(S11)</f>
+        <f t="shared" si="11"/>
         <v>6.2632412710493526</v>
       </c>
       <c r="U11" t="s">
@@ -6692,39 +6757,39 @@
         <v>1.3987330927951678</v>
       </c>
       <c r="K12" s="1">
-        <f>(F12/$F$2)/(C12/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>4.6688614913277657</v>
       </c>
       <c r="M12">
-        <f>(D12-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.14263412188717953</v>
       </c>
       <c r="N12">
-        <f>(E12-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.9770025041115533</v>
       </c>
       <c r="O12">
-        <f>(F12-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.3142480493147989E-2</v>
       </c>
       <c r="P12">
-        <f>(G12-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>1.3607433484156346</v>
       </c>
       <c r="Q12">
-        <f>(H12-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.2158104647259057</v>
       </c>
       <c r="R12">
-        <f>(I12-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.5722309760090816</v>
       </c>
       <c r="S12">
-        <f>(J12-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.52305664619539227</v>
       </c>
       <c r="T12">
-        <f>ABS(M12)+ABS(N12)+ABS(O12)+ABS(P12)+ABS(Q12)+ABS(R12)+ABS(S12)</f>
+        <f t="shared" si="11"/>
         <v>5.8046205418378953</v>
       </c>
       <c r="U12" t="s">
@@ -6766,39 +6831,39 @@
         <v>1.254635780674259</v>
       </c>
       <c r="K13" s="1">
-        <f>(F13/$F$2)/(C13/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>3.5212482087265888</v>
       </c>
       <c r="M13">
-        <f>(D13-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.41176642066684982</v>
       </c>
       <c r="N13">
-        <f>(E13-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.0918517716106275</v>
       </c>
       <c r="O13">
-        <f>(F13-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.87880161598430973</v>
       </c>
       <c r="P13">
-        <f>(G13-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.83929060540964306</v>
       </c>
       <c r="Q13">
-        <f>(H13-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.31219183732194145</v>
       </c>
       <c r="R13">
-        <f>(I13-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.1443668227107135</v>
       </c>
       <c r="S13">
-        <f>(J13-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.3340303071088298</v>
       </c>
       <c r="T13">
-        <f>ABS(M13)+ABS(N13)+ABS(O13)+ABS(P13)+ABS(Q13)+ABS(R13)+ABS(S13)</f>
+        <f t="shared" si="11"/>
         <v>5.012299380812915</v>
       </c>
       <c r="U13" t="s">
@@ -6840,39 +6905,39 @@
         <v>1.2793778471339445</v>
       </c>
       <c r="K14" s="1">
-        <f>(F14/$F$2)/(C14/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>3.4879840556077149</v>
       </c>
       <c r="M14">
-        <f>(D14-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.43261776850627126</v>
       </c>
       <c r="N14">
-        <f>(E14-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.134879932218311</v>
       </c>
       <c r="O14">
-        <f>(F14-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.86414716870876407</v>
       </c>
       <c r="P14">
-        <f>(G14-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.81973612754691849</v>
       </c>
       <c r="Q14">
-        <f>(H14-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.28032962943974377</v>
       </c>
       <c r="R14">
-        <f>(I14-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.0730561304943191</v>
       </c>
       <c r="S14">
-        <f>(J14-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.36648686147111037</v>
       </c>
       <c r="T14">
-        <f>ABS(M14)+ABS(N14)+ABS(O14)+ABS(P14)+ABS(Q14)+ABS(R14)+ABS(S14)</f>
+        <f t="shared" si="11"/>
         <v>4.9712536183854388</v>
       </c>
       <c r="U14" t="s">
@@ -6914,39 +6979,39 @@
         <v>3.3099850113629325</v>
       </c>
       <c r="K15" s="1">
-        <f>(F15/$F$2)/(C15/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>3.1933586994119678</v>
       </c>
       <c r="M15">
-        <f>(D15-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.57413436717591304</v>
       </c>
       <c r="N15">
-        <f>(E15-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.36188536892040751</v>
       </c>
       <c r="O15">
-        <f>(F15-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.43800514634686505</v>
       </c>
       <c r="P15">
-        <f>(G15-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.68937294179542064</v>
       </c>
       <c r="Q15">
-        <f>(H15-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.516225567615198</v>
       </c>
       <c r="R15">
-        <f>(I15-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.35315771383357369</v>
       </c>
       <c r="S15">
-        <f>(J15-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>3.0302300828233699</v>
       </c>
       <c r="T15">
-        <f>ABS(M15)+ABS(N15)+ABS(O15)+ABS(P15)+ABS(Q15)+ABS(R15)+ABS(S15)</f>
+        <f t="shared" si="11"/>
         <v>5.9630111885107482</v>
       </c>
       <c r="U15" t="s">
@@ -6988,39 +7053,39 @@
         <v>0.76439566985384333</v>
       </c>
       <c r="K16" s="1">
-        <f>(F16/$F$2)/(C16/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>2.4805554182932252</v>
       </c>
       <c r="M16">
-        <f>(D16-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.57977649659128594</v>
       </c>
       <c r="N16">
-        <f>(E16-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.43257448991874536</v>
       </c>
       <c r="O16">
-        <f>(F16-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.4903424580452424</v>
       </c>
       <c r="P16">
-        <f>(G16-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.36346497741667599</v>
       </c>
       <c r="Q16">
-        <f>(H16-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.39788022405274959</v>
       </c>
       <c r="R16">
-        <f>(I16-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.5009202837926872</v>
       </c>
       <c r="S16">
-        <f>(J16-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.30906491831784533</v>
       </c>
       <c r="T16">
-        <f>ABS(M16)+ABS(N16)+ABS(O16)+ABS(P16)+ABS(Q16)+ABS(R16)+ABS(S16)</f>
+        <f t="shared" si="11"/>
         <v>4.0740238481352318</v>
       </c>
       <c r="U16" t="s">
@@ -7062,39 +7127,39 @@
         <v>0.74305785969371951</v>
       </c>
       <c r="K17" s="1">
-        <f>(F17/$F$2)/(C17/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>2.2857225214541015</v>
       </c>
       <c r="M17">
-        <f>(D17-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.30282153528885269</v>
       </c>
       <c r="N17">
-        <f>(E17-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>0.28661048023825703</v>
       </c>
       <c r="O17">
-        <f>(F17-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.16899136421720537</v>
       </c>
       <c r="P17">
-        <f>(G17-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.27221074739062756</v>
       </c>
       <c r="Q17">
-        <f>(H17-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-7.9258145230772889E-2</v>
       </c>
       <c r="R17">
-        <f>(I17-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.3582988993598977</v>
       </c>
       <c r="S17">
-        <f>(J17-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.33705578143198811</v>
       </c>
       <c r="T17">
-        <f>ABS(M17)+ABS(N17)+ABS(O17)+ABS(P17)+ABS(Q17)+ABS(R17)+ABS(S17)</f>
+        <f t="shared" si="11"/>
         <v>2.8052469531576012</v>
       </c>
       <c r="U17" t="s">
@@ -7136,39 +7201,39 @@
         <v>2.3731410393968169</v>
       </c>
       <c r="K18" s="1">
-        <f>(F18/$F$2)/(C18/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>2.081385580866729</v>
       </c>
       <c r="M18">
-        <f>(D18-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.58689048585414738</v>
       </c>
       <c r="N18">
-        <f>(E18-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.52170425117751917</v>
       </c>
       <c r="O18">
-        <f>(F18-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.51965135259633377</v>
       </c>
       <c r="P18">
-        <f>(G18-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.18095651736457891</v>
       </c>
       <c r="Q18">
-        <f>(H18-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.52077731159836915</v>
       </c>
       <c r="R18">
-        <f>(I18-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.42446840604996833</v>
       </c>
       <c r="S18">
-        <f>(J18-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>1.8012815083525413</v>
       </c>
       <c r="T18">
-        <f>ABS(M18)+ABS(N18)+ABS(O18)+ABS(P18)+ABS(Q18)+ABS(R18)+ABS(S18)</f>
+        <f t="shared" si="11"/>
         <v>4.5557298329934577</v>
       </c>
       <c r="U18" t="s">
@@ -7210,39 +7275,39 @@
         <v>1.5170764635413443</v>
       </c>
       <c r="K19" s="1">
-        <f>(F19/$F$2)/(C19/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.9958491871324802</v>
       </c>
       <c r="M19">
-        <f>(D19-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.57339843725216877</v>
       </c>
       <c r="N19">
-        <f>(E19-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.35266504879018956</v>
       </c>
       <c r="O19">
-        <f>(F19-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.52593183000013899</v>
       </c>
       <c r="P19">
-        <f>(G19-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.14184756163912957</v>
       </c>
       <c r="Q19">
-        <f>(H19-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.49801859168251367</v>
       </c>
       <c r="R19">
-        <f>(I19-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-6.7914944967995217E-2</v>
       </c>
       <c r="S19">
-        <f>(J19-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.67829905702220461</v>
       </c>
       <c r="T19">
-        <f>ABS(M19)+ABS(N19)+ABS(O19)+ABS(P19)+ABS(Q19)+ABS(R19)+ABS(S19)</f>
+        <f t="shared" si="11"/>
         <v>2.8380754713543404</v>
       </c>
       <c r="U19" t="s">
@@ -7284,39 +7349,39 @@
         <v>1.2190793010600087</v>
       </c>
       <c r="K20" s="1">
-        <f>(F20/$F$2)/(C20/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.9245688590206054</v>
       </c>
       <c r="M20">
-        <f>(D20-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.56849223776054014</v>
       </c>
       <c r="N20">
-        <f>(E20-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.29119624792206966</v>
       </c>
       <c r="O20">
-        <f>(F20-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.53116556116997682</v>
       </c>
       <c r="P20">
-        <f>(G20-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>0.1092567652012552</v>
       </c>
       <c r="Q20">
-        <f>(H20-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.48436335973300038</v>
       </c>
       <c r="R20">
-        <f>(I20-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.14601713168118866</v>
       </c>
       <c r="S20">
-        <f>(J20-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.28738744421734036</v>
       </c>
       <c r="T20">
-        <f>ABS(M20)+ABS(N20)+ABS(O20)+ABS(P20)+ABS(Q20)+ABS(R20)+ABS(S20)</f>
+        <f t="shared" si="11"/>
         <v>2.4178787476853714</v>
       </c>
       <c r="U20" t="s">
@@ -7358,39 +7423,39 @@
         <v>0.96752325480953072</v>
       </c>
       <c r="K21" s="1">
-        <f>(F21/$F$2)/(C21/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.7855722192024508</v>
       </c>
       <c r="M21">
-        <f>(D21-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.28957479666145547</v>
       </c>
       <c r="N21">
-        <f>(E21-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-1.4586644015530316E-2</v>
       </c>
       <c r="O21">
-        <f>(F21-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.14805643953785438</v>
       </c>
       <c r="P21">
-        <f>(G21-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>4.4075172325506298E-2</v>
       </c>
       <c r="Q21">
-        <f>(H21-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.17939651286053698</v>
       </c>
       <c r="R21">
-        <f>(I21-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.35994920833037264</v>
       </c>
       <c r="S21">
-        <f>(J21-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-4.2602878280272191E-2</v>
       </c>
       <c r="T21">
-        <f>ABS(M21)+ABS(N21)+ABS(O21)+ABS(P21)+ABS(Q21)+ABS(R21)+ABS(S21)</f>
+        <f t="shared" si="11"/>
         <v>1.0782416520115281</v>
       </c>
       <c r="U21" t="s">
@@ -7432,39 +7497,39 @@
         <v>0.91615656564509751</v>
       </c>
       <c r="K22" s="1">
-        <f>(F22/$F$2)/(C22/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.772504159048607</v>
       </c>
       <c r="M22">
-        <f>(D22-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.17673220835399817</v>
       </c>
       <c r="N22">
-        <f>(E22-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>0.81216872766068204</v>
       </c>
       <c r="O22">
-        <f>(F22-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.28203995748570049</v>
       </c>
       <c r="P22">
-        <f>(G22-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>3.7557013037931325E-2</v>
       </c>
       <c r="Q22">
-        <f>(H22-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.26132790455761667</v>
       </c>
       <c r="R22">
-        <f>(I22-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.43125990054676738</v>
       </c>
       <c r="S22">
-        <f>(J22-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.10998551755950488</v>
       </c>
       <c r="T22">
-        <f>ABS(M22)+ABS(N22)+ABS(O22)+ABS(P22)+ABS(Q22)+ABS(R22)+ABS(S22)</f>
+        <f t="shared" si="11"/>
         <v>2.1110712292022011</v>
       </c>
       <c r="U22" t="s">
@@ -7506,39 +7571,39 @@
         <v>1.7879829748880127</v>
       </c>
       <c r="K23" s="1">
-        <f>(F23/$F$2)/(C23/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.732111973118545</v>
       </c>
       <c r="M23">
-        <f>(D23-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.46717921825841002</v>
       </c>
       <c r="N23">
-        <f>(E23-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-5.4541364579808203E-2</v>
       </c>
       <c r="O23">
-        <f>(F23-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.41811696790148167</v>
       </c>
       <c r="P23">
-        <f>(G23-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>1.8002535175206742E-2</v>
       </c>
       <c r="Q23">
-        <f>(H23-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.46160463981714495</v>
       </c>
       <c r="R23">
-        <f>(I23-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.35315771383357369</v>
       </c>
       <c r="S23">
-        <f>(J23-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>1.0336732504811716</v>
       </c>
       <c r="T23">
-        <f>ABS(M23)+ABS(N23)+ABS(O23)+ABS(P23)+ABS(Q23)+ABS(R23)+ABS(S23)</f>
+        <f t="shared" si="11"/>
         <v>2.8062756900467969</v>
       </c>
       <c r="U23" t="s">
@@ -7580,39 +7645,39 @@
         <v>1.5170764635413443</v>
       </c>
       <c r="K24" s="1">
-        <f>(F24/$F$2)/(C24/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.6029163784157729</v>
       </c>
       <c r="M24">
-        <f>(D24-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.54129008724584426</v>
       </c>
       <c r="N24">
-        <f>(E24-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.1713320862292359</v>
       </c>
       <c r="O24">
-        <f>(F24-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.2106201721520224</v>
       </c>
       <c r="P24">
-        <f>(G24-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-4.0660898412967356E-2</v>
       </c>
       <c r="Q24">
-        <f>(H24-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.32129532528828358</v>
       </c>
       <c r="R24">
-        <f>(I24-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.28184702161717912</v>
       </c>
       <c r="S24">
-        <f>(J24-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.67829905702220461</v>
       </c>
       <c r="T24">
-        <f>ABS(M24)+ABS(N24)+ABS(O24)+ABS(P24)+ABS(Q24)+ABS(R24)+ABS(S24)</f>
+        <f t="shared" si="11"/>
         <v>3.2453446479677375</v>
       </c>
       <c r="U24" t="s">
@@ -7654,39 +7719,39 @@
         <v>0.75618252297635324</v>
       </c>
       <c r="K25" s="1">
-        <f>(F25/$F$2)/(C25/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.5282502347185847</v>
       </c>
       <c r="M25">
-        <f>(D25-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.67571995331646739</v>
       </c>
       <c r="N25">
-        <f>(E25-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>3.8539962449056979E-3</v>
       </c>
       <c r="O25">
-        <f>(F25-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>1.0106916414642209</v>
       </c>
       <c r="P25">
-        <f>(G25-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-7.3251694850841806E-2</v>
       </c>
       <c r="Q25">
-        <f>(H25-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>1.0268156426798034</v>
       </c>
       <c r="R25">
-        <f>(I25-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.50257059276316185</v>
       </c>
       <c r="S25">
-        <f>(J25-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.3198388950408082</v>
       </c>
       <c r="T25">
-        <f>ABS(M25)+ABS(N25)+ABS(O25)+ABS(P25)+ABS(Q25)+ABS(R25)+ABS(S25)</f>
+        <f t="shared" si="11"/>
         <v>3.6127424163602093</v>
       </c>
       <c r="U25" t="s">
@@ -7728,39 +7793,39 @@
         <v>0.89826895867579581</v>
       </c>
       <c r="K26" s="1">
-        <f>(F26/$F$2)/(C26/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.5040149231605473</v>
       </c>
       <c r="M26">
-        <f>(D26-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>5.0424828108405005E-2</v>
       </c>
       <c r="N26">
-        <f>(E26-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-2.073352410234228E-2</v>
       </c>
       <c r="O26">
-        <f>(F26-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.21097751871301437</v>
       </c>
       <c r="P26">
-        <f>(G26-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-8.6288013425991669E-2</v>
       </c>
       <c r="Q26">
-        <f>(H26-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.15288079791095308</v>
       </c>
       <c r="R26">
-        <f>(I26-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.2173278238975834</v>
       </c>
       <c r="S26">
-        <f>(J26-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.13345041645775266</v>
       </c>
       <c r="T26">
-        <f>ABS(M26)+ABS(N26)+ABS(O26)+ABS(P26)+ABS(Q26)+ABS(R26)+ABS(S26)</f>
+        <f t="shared" si="11"/>
         <v>0.87208292261604259</v>
       </c>
       <c r="U26" t="s">
@@ -7802,39 +7867,39 @@
         <v>0.43026328272706188</v>
       </c>
       <c r="K27" s="1">
-        <f>(F27/$F$2)/(C27/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.2830459060137371</v>
       </c>
       <c r="M27">
-        <f>(D27-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.38745347651944567</v>
       </c>
       <c r="N27">
-        <f>(E27-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>1.9770025041115533</v>
       </c>
       <c r="O27">
-        <f>(F27-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.5782691416985164</v>
       </c>
       <c r="P27">
-        <f>(G27-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.18406040273961502</v>
       </c>
       <c r="Q27">
-        <f>(H27-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.41153545600226288</v>
       </c>
       <c r="R27">
-        <f>(I27-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>1.286988207143503</v>
       </c>
       <c r="S27">
-        <f>(J27-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.74737858967788806</v>
       </c>
       <c r="T27">
-        <f>ABS(M27)+ABS(N27)+ABS(O27)+ABS(P27)+ABS(Q27)+ABS(R27)+ABS(S27)</f>
+        <f t="shared" si="11"/>
         <v>5.572687777892785</v>
       </c>
       <c r="U27" t="s">
@@ -7876,39 +7941,39 @@
         <v>0.7151931899552052</v>
       </c>
       <c r="K28" s="1">
-        <f>(F28/$F$2)/(C28/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.2545337747689875</v>
       </c>
       <c r="M28">
-        <f>(D28-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.48655870625034287</v>
       </c>
       <c r="N28">
-        <f>(E28-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>0.73533272657553217</v>
       </c>
       <c r="O28">
-        <f>(F28-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.58036263416645151</v>
       </c>
       <c r="P28">
-        <f>(G28-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.1970967213147648</v>
       </c>
       <c r="Q28">
-        <f>(H28-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.47525987176665824</v>
       </c>
       <c r="R28">
-        <f>(I28-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.28863851611397817</v>
       </c>
       <c r="S28">
-        <f>(J28-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.37360855561633877</v>
       </c>
       <c r="T28">
-        <f>ABS(M28)+ABS(N28)+ABS(O28)+ABS(P28)+ABS(Q28)+ABS(R28)+ABS(S28)</f>
+        <f t="shared" si="11"/>
         <v>3.1368577318040662</v>
       </c>
       <c r="U28" t="s">
@@ -7950,39 +8015,39 @@
         <v>1.2028249103792086</v>
       </c>
       <c r="K29" s="1">
-        <f>(F29/$F$2)/(C29/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.0549488560557396</v>
       </c>
       <c r="M29">
-        <f>(D29-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.54984867969235163</v>
       </c>
       <c r="N29">
-        <f>(E29-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-5.7614804623214187E-2</v>
       </c>
       <c r="O29">
-        <f>(F29-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.59501708144199716</v>
       </c>
       <c r="P29">
-        <f>(G29-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.28835095134081334</v>
       </c>
       <c r="Q29">
-        <f>(H29-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.52077731159836915</v>
       </c>
       <c r="R29">
-        <f>(I29-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.42446840604996833</v>
       </c>
       <c r="S29">
-        <f>(J29-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.26606499260980226</v>
       </c>
       <c r="T29">
-        <f>ABS(M29)+ABS(N29)+ABS(O29)+ABS(P29)+ABS(Q29)+ABS(R29)+ABS(S29)</f>
+        <f t="shared" si="11"/>
         <v>2.7021422273565165</v>
       </c>
       <c r="U29" t="s">
@@ -8024,39 +8089,39 @@
         <v>0.91274655361416024</v>
       </c>
       <c r="K30" s="1">
-        <f>(F30/$F$2)/(C30/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>1.0406927904333645</v>
       </c>
       <c r="M30">
-        <f>(D30-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.50986315383557868</v>
       </c>
       <c r="N30">
-        <f>(E30-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.32193064835612961</v>
       </c>
       <c r="O30">
-        <f>(F30-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.51965135259633377</v>
       </c>
       <c r="P30">
-        <f>(G30-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.29486911062838822</v>
       </c>
       <c r="Q30">
-        <f>(H30-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.44339766388446056</v>
       </c>
       <c r="R30">
-        <f>(I30-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.21053632940078446</v>
       </c>
       <c r="S30">
-        <f>(J30-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.11445875915549213</v>
       </c>
       <c r="T30">
-        <f>ABS(M30)+ABS(N30)+ABS(O30)+ABS(P30)+ABS(Q30)+ABS(R30)+ABS(S30)</f>
+        <f t="shared" si="11"/>
         <v>2.4147070178571672</v>
       </c>
       <c r="U30" t="s">
@@ -8098,39 +8163,39 @@
         <v>0.50240843922473089</v>
       </c>
       <c r="K31" s="1">
-        <f>(F31/$F$2)/(C31/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>0.97297647872708393</v>
       </c>
       <c r="M31">
-        <f>(D31-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.38254727702781705</v>
       </c>
       <c r="N31">
-        <f>(E31-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.30656344813909958</v>
       </c>
       <c r="O31">
-        <f>(F31-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.38671458088245519</v>
       </c>
       <c r="P31">
-        <f>(G31-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.32745990706626266</v>
       </c>
       <c r="Q31">
-        <f>(H31-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.15208604896151043</v>
       </c>
       <c r="R31">
-        <f>(I31-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.43125990054676738</v>
       </c>
       <c r="S31">
-        <f>(J31-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.65273883120592779</v>
       </c>
       <c r="T31">
-        <f>ABS(M31)+ABS(N31)+ABS(O31)+ABS(P31)+ABS(Q31)+ABS(R31)+ABS(S31)</f>
+        <f t="shared" si="11"/>
         <v>2.6393699938298401</v>
       </c>
       <c r="U31" t="s">
@@ -8172,39 +8237,39 @@
         <v>0.42113648582073027</v>
       </c>
       <c r="K32" s="1">
-        <f>(F32/$F$2)/(C32/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>0.81588560177283787</v>
       </c>
       <c r="M32">
-        <f>(D32-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>0.25280555713808395</v>
       </c>
       <c r="N32">
-        <f>(E32-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.23587432714076176</v>
       </c>
       <c r="O32">
-        <f>(F32-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>0.10630289531625965</v>
       </c>
       <c r="P32">
-        <f>(G32-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.39915965922958646</v>
       </c>
       <c r="Q32">
-        <f>(H32-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>0.78102146758856406</v>
       </c>
       <c r="R32">
-        <f>(I32-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>0.43125990054676738</v>
       </c>
       <c r="S32">
-        <f>(J32-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.75935108924361805</v>
       </c>
       <c r="T32">
-        <f>ABS(M32)+ABS(N32)+ABS(O32)+ABS(P32)+ABS(Q32)+ABS(R32)+ABS(S32)</f>
+        <f t="shared" si="11"/>
         <v>2.9657748962036412</v>
       </c>
       <c r="U32" t="s">
@@ -8246,39 +8311,39 @@
         <v>1.2539101382331519</v>
       </c>
       <c r="K33" s="1">
-        <f>(F33/$F$2)/(C33/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>0.76982754360824235</v>
       </c>
       <c r="M33">
-        <f>(D33-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.55524549913314303</v>
       </c>
       <c r="N33">
-        <f>(E33-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.12523048557814603</v>
       </c>
       <c r="O33">
-        <f>(F33-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.61595200612134815</v>
       </c>
       <c r="P33">
-        <f>(G33-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.41871413709231114</v>
       </c>
       <c r="Q33">
-        <f>(H33-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.5344325435478825</v>
       </c>
       <c r="R33">
-        <f>(I33-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S33">
-        <f>(J33-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.3330784119477791</v>
       </c>
       <c r="T33">
-        <f>ABS(M33)+ABS(N33)+ABS(O33)+ABS(P33)+ABS(Q33)+ABS(R33)+ABS(S33)</f>
+        <f t="shared" si="11"/>
         <v>3.2210535661197626</v>
       </c>
       <c r="U33" t="s">
@@ -8320,39 +8385,39 @@
         <v>1.1145867895405792</v>
       </c>
       <c r="K34" s="1">
-        <f>(F34/$F$2)/(C34/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>0.6842911498739932</v>
       </c>
       <c r="M34">
-        <f>(D34-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.60725121374440594</v>
       </c>
       <c r="N34">
-        <f>(E34-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.77679977478021667</v>
       </c>
       <c r="O34">
-        <f>(F34-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.62223248352515348</v>
       </c>
       <c r="P34">
-        <f>(G34-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.45782309281776046</v>
       </c>
       <c r="Q34">
-        <f>(H34-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.5344325435478825</v>
       </c>
       <c r="R34">
-        <f>(I34-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S34">
-        <f>(J34-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>0.15031454102602415</v>
       </c>
       <c r="T34">
-        <f>ABS(M34)+ABS(N34)+ABS(O34)+ABS(P34)+ABS(Q34)+ABS(R34)+ABS(S34)</f>
+        <f t="shared" si="11"/>
         <v>3.7872541321405957</v>
       </c>
       <c r="U34" t="s">
@@ -8394,39 +8459,39 @@
         <v>0.91430947579500654</v>
       </c>
       <c r="K35" s="1">
-        <f>(F35/$F$2)/(C35/$C$2)</f>
+        <f t="shared" si="3"/>
         <v>0.64541097090388</v>
       </c>
       <c r="M35">
-        <f>(D35-$M$2)/$M$1</f>
+        <f t="shared" si="4"/>
         <v>-0.13969040219220238</v>
       </c>
       <c r="N35">
-        <f>(E35-$N$2)/$N$1</f>
+        <f t="shared" si="5"/>
         <v>-0.52785113126433114</v>
       </c>
       <c r="O35">
-        <f>(F35-$O$2)/$O$1</f>
+        <f t="shared" si="6"/>
         <v>-0.15119667823975699</v>
       </c>
       <c r="P35">
-        <f>(G35-$P$2)/$P$1</f>
+        <f t="shared" si="7"/>
         <v>-0.47737757068048525</v>
       </c>
       <c r="Q35">
-        <f>(H35-$Q$2)/$Q$1</f>
+        <f t="shared" si="8"/>
         <v>-0.15663779294468153</v>
       </c>
       <c r="R35">
-        <f>(I35-$R$2)/$R$1</f>
+        <f t="shared" si="9"/>
         <v>-0.56708979048275776</v>
       </c>
       <c r="S35">
-        <f>(J35-$S$2)/$S$1</f>
+        <f t="shared" si="10"/>
         <v>-0.1124085234239979</v>
       </c>
       <c r="T35">
-        <f>ABS(M35)+ABS(N35)+ABS(O35)+ABS(P35)+ABS(Q35)+ABS(R35)+ABS(S35)</f>
+        <f t="shared" si="11"/>
         <v>2.132251889228213</v>
       </c>
       <c r="U35" t="s">
@@ -8468,39 +8533,39 @@
         <v>0.59106875202909515</v>
       </c>
       <c r="K36" s="1">
-        <f>(F36/$F$2)/(C36/$C$2)</f>
+        <f t="shared" ref="K36:K66" si="12">(F36/$F$2)/(C36/$C$2)</f>
         <v>0.58190667858602829</v>
       </c>
       <c r="M36">
-        <f>(D36-$M$2)/$M$1</f>
+        <f t="shared" ref="M36:M66" si="13">(D36-$M$2)/$M$1</f>
         <v>-0.19169611680346532</v>
       </c>
       <c r="N36">
-        <f>(E36-$N$2)/$N$1</f>
+        <f t="shared" ref="N36:N66" si="14">(E36-$N$2)/$N$1</f>
         <v>-0.58624649208904511</v>
       </c>
       <c r="O36">
-        <f>(F36-$O$2)/$O$1</f>
+        <f t="shared" ref="O36:O66" si="15">(F36-$O$2)/$O$1</f>
         <v>-0.20248724370416685</v>
       </c>
       <c r="P36">
-        <f>(G36-$P$2)/$P$1</f>
+        <f t="shared" ref="P36:P66" si="16">(G36-$P$2)/$P$1</f>
         <v>-0.50996836711835958</v>
       </c>
       <c r="Q36">
-        <f>(H36-$Q$2)/$Q$1</f>
+        <f t="shared" ref="Q36:Q66" si="17">(H36-$Q$2)/$Q$1</f>
         <v>1.6328478415820181E-2</v>
       </c>
       <c r="R36">
-        <f>(I36-$R$2)/$R$1</f>
+        <f t="shared" ref="R36:R66" si="18">(I36-$R$2)/$R$1</f>
         <v>-0.35315771383357369</v>
       </c>
       <c r="S36">
-        <f>(J36-$S$2)/$S$1</f>
+        <f t="shared" ref="S36:S66" si="19">(J36-$S$2)/$S$1</f>
         <v>-0.53643454971026572</v>
       </c>
       <c r="T36">
-        <f>ABS(M36)+ABS(N36)+ABS(O36)+ABS(P36)+ABS(Q36)+ABS(R36)+ABS(S36)</f>
+        <f t="shared" ref="T36:T67" si="20">ABS(M36)+ABS(N36)+ABS(O36)+ABS(P36)+ABS(Q36)+ABS(R36)+ABS(S36)</f>
         <v>2.3963189616746963</v>
       </c>
       <c r="U36" t="s">
@@ -8542,39 +8607,39 @@
         <v>0.46262496553046484</v>
       </c>
       <c r="K37" s="1">
-        <f>(F37/$F$2)/(C37/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.52747442802786981</v>
       </c>
       <c r="M37">
-        <f>(D37-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.58885296565079881</v>
       </c>
       <c r="N37">
-        <f>(E37-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.54629177152476716</v>
       </c>
       <c r="O37">
-        <f>(F37-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.63374669209879642</v>
       </c>
       <c r="P37">
-        <f>(G37-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.52952284498108437</v>
       </c>
       <c r="Q37">
-        <f>(H37-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.50712207964885592</v>
       </c>
       <c r="R37">
-        <f>(I37-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.21053632940078446</v>
       </c>
       <c r="S37">
-        <f>(J37-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.70492664982577613</v>
       </c>
       <c r="T37">
-        <f>ABS(M37)+ABS(N37)+ABS(O37)+ABS(P37)+ABS(Q37)+ABS(R37)+ABS(S37)</f>
+        <f t="shared" si="20"/>
         <v>3.7209993331308628</v>
       </c>
       <c r="U37" t="s">
@@ -8616,39 +8681,39 @@
         <v>0.43761821063692624</v>
       </c>
       <c r="K38" s="1">
-        <f>(F38/$F$2)/(C38/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.51007941217671515</v>
       </c>
       <c r="M38">
-        <f>(D38-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>5.0422375008659026</v>
       </c>
       <c r="N38">
-        <f>(E38-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.43564792996215135</v>
       </c>
       <c r="O38">
-        <f>(F38-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>3.4098340097178399</v>
       </c>
       <c r="P38">
-        <f>(G38-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.54255916355623413</v>
       </c>
       <c r="Q38">
-        <f>(H38-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>6.083803207982891</v>
       </c>
       <c r="R38">
-        <f>(I38-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.21053632940078446</v>
       </c>
       <c r="S38">
-        <f>(J38-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.73773042152968071</v>
       </c>
       <c r="T38">
-        <f>ABS(M38)+ABS(N38)+ABS(O38)+ABS(P38)+ABS(Q38)+ABS(R38)+ABS(S38)</f>
+        <f t="shared" si="20"/>
         <v>16.462348563015485</v>
       </c>
       <c r="U38" t="s">
@@ -8690,39 +8755,39 @@
         <v>0.47285500162327609</v>
       </c>
       <c r="K39" s="1">
-        <f>(F39/$F$2)/(C39/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.4668861491327766</v>
       </c>
       <c r="M39">
-        <f>(D39-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.51869431292051016</v>
       </c>
       <c r="N39">
-        <f>(E39-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.73377161417253267</v>
       </c>
       <c r="O39">
-        <f>(F39-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.53535254610584693</v>
       </c>
       <c r="P39">
-        <f>(G39-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.56211364141895881</v>
       </c>
       <c r="Q39">
-        <f>(H39-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.35691452820420971</v>
       </c>
       <c r="R39">
-        <f>(I39-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.35315771383357369</v>
       </c>
       <c r="S39">
-        <f>(J39-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.69150692503781519</v>
       </c>
       <c r="T39">
-        <f>ABS(M39)+ABS(N39)+ABS(O39)+ABS(P39)+ABS(Q39)+ABS(R39)+ABS(S39)</f>
+        <f t="shared" si="20"/>
         <v>3.7515112816934471</v>
       </c>
       <c r="U39" t="s">
@@ -8764,39 +8829,39 @@
         <v>0.55987345678311518</v>
       </c>
       <c r="K40" s="1">
-        <f>(F40/$F$2)/(C40/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.44906606710480801</v>
       </c>
       <c r="M40">
-        <f>(D40-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.57266250732842439</v>
       </c>
       <c r="N40">
-        <f>(E40-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.71533097391209677</v>
       </c>
       <c r="O40">
-        <f>(F40-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.60653129001564021</v>
       </c>
       <c r="P40">
-        <f>(G40-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.56863180070653374</v>
       </c>
       <c r="Q40">
-        <f>(H40-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.48436335973300038</v>
       </c>
       <c r="R40">
-        <f>(I40-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.49577909826636307</v>
       </c>
       <c r="S40">
-        <f>(J40-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.57735642653281338</v>
       </c>
       <c r="T40">
-        <f>ABS(M40)+ABS(N40)+ABS(O40)+ABS(P40)+ABS(Q40)+ABS(R40)+ABS(S40)</f>
+        <f t="shared" si="20"/>
         <v>4.0206554564948718</v>
       </c>
       <c r="U40" t="s">
@@ -8838,39 +8903,39 @@
         <v>0.71983730157829084</v>
       </c>
       <c r="K41" s="1">
-        <f>(F41/$F$2)/(C41/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.44193803429362061</v>
       </c>
       <c r="M41">
-        <f>(D41-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.45859336914806004</v>
       </c>
       <c r="N41">
-        <f>(E41-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-2.2928838419062668E-3</v>
       </c>
       <c r="O41">
-        <f>(F41-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.60757803624960782</v>
       </c>
       <c r="P41">
-        <f>(G41-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.56863180070653374</v>
       </c>
       <c r="Q41">
-        <f>(H41-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.50257033566568476</v>
       </c>
       <c r="R41">
-        <f>(I41-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S41">
-        <f>(J41-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.36751642658561379</v>
       </c>
       <c r="T41">
-        <f>ABS(M41)+ABS(N41)+ABS(O41)+ABS(P41)+ABS(Q41)+ABS(R41)+ABS(S41)</f>
+        <f t="shared" si="20"/>
         <v>3.1455833348965592</v>
       </c>
       <c r="U41" t="s">
@@ -8912,39 +8977,39 @@
         <v>1.2190793010600087</v>
       </c>
       <c r="K42" s="1">
-        <f>(F42/$F$2)/(C42/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.43481000148243309</v>
       </c>
       <c r="M42">
-        <f>(D42-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.32857908261990265</v>
       </c>
       <c r="N42">
-        <f>(E42-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.13752424575176997</v>
       </c>
       <c r="O42">
-        <f>(F42-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.54477326221155487</v>
       </c>
       <c r="P42">
-        <f>(G42-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.57514995999410856</v>
       </c>
       <c r="Q42">
-        <f>(H42-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.49346684769934257</v>
       </c>
       <c r="R42">
-        <f>(I42-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.85233255934833629</v>
       </c>
       <c r="S42">
-        <f>(J42-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>0.28738744421734036</v>
       </c>
       <c r="T42">
-        <f>ABS(M42)+ABS(N42)+ABS(O42)+ABS(P42)+ABS(Q42)+ABS(R42)+ABS(S42)</f>
+        <f t="shared" si="20"/>
         <v>3.2192134018423553</v>
       </c>
       <c r="U42" t="s">
@@ -8986,39 +9051,39 @@
         <v>0.56890367382800411</v>
       </c>
       <c r="K43" s="1">
-        <f>(F43/$F$2)/(C43/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.39916983742649598</v>
       </c>
       <c r="M43">
-        <f>(D43-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.5419987605057458</v>
       </c>
       <c r="N43">
-        <f>(E43-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>4.0735276765777484E-2</v>
       </c>
       <c r="O43">
-        <f>(F43-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.64316740820450435</v>
       </c>
       <c r="P43">
-        <f>(G43-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.58818627856925831</v>
       </c>
       <c r="Q43">
-        <f>(H43-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.52988079956471135</v>
       </c>
       <c r="R43">
-        <f>(I43-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.56708979048275776</v>
       </c>
       <c r="S43">
-        <f>(J43-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.56551062008418118</v>
       </c>
       <c r="T43">
-        <f>ABS(M43)+ABS(N43)+ABS(O43)+ABS(P43)+ABS(Q43)+ABS(R43)+ABS(S43)</f>
+        <f t="shared" si="20"/>
         <v>3.4765689341769357</v>
       </c>
       <c r="U43" t="s">
@@ -9060,39 +9125,39 @@
         <v>0.73144758063600523</v>
       </c>
       <c r="K44" s="1">
-        <f>(F44/$F$2)/(C44/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.38610177727265238</v>
       </c>
       <c r="M44">
-        <f>(D44-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>1.4661086914178314</v>
       </c>
       <c r="N44">
-        <f>(E44-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.35881192887700153</v>
       </c>
       <c r="O44">
-        <f>(F44-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>0.3481012753627632</v>
       </c>
       <c r="P44">
-        <f>(G44-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.59470443785683325</v>
       </c>
       <c r="Q44">
-        <f>(H44-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>0.57619298834586496</v>
       </c>
       <c r="R44">
-        <f>(I44-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.70971117491554692</v>
       </c>
       <c r="S44">
-        <f>(J44-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.35228610400880084</v>
       </c>
       <c r="T44">
-        <f>ABS(M44)+ABS(N44)+ABS(O44)+ABS(P44)+ABS(Q44)+ABS(R44)+ABS(S44)</f>
+        <f t="shared" si="20"/>
         <v>4.405916600784642</v>
       </c>
       <c r="U44" t="s">
@@ -9134,39 +9199,39 @@
         <v>2.1943427419080157</v>
       </c>
       <c r="K45" s="1">
-        <f>(F45/$F$2)/(C45/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.38491377180412117</v>
       </c>
       <c r="M45">
-        <f>(D45-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.62368698204136175</v>
       </c>
       <c r="N45">
-        <f>(E45-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-1.03496873842632</v>
       </c>
       <c r="O45">
-        <f>(F45-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.61595200612134815</v>
       </c>
       <c r="P45">
-        <f>(G45-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.59470443785683325</v>
       </c>
       <c r="Q45">
-        <f>(H45-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.54808777549739573</v>
       </c>
       <c r="R45">
-        <f>(I45-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.99495394378112556</v>
       </c>
       <c r="S45">
-        <f>(J45-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>1.5667345406696229</v>
       </c>
       <c r="T45">
-        <f>ABS(M45)+ABS(N45)+ABS(O45)+ABS(P45)+ABS(Q45)+ABS(R45)+ABS(S45)</f>
+        <f t="shared" si="20"/>
         <v>5.9790884243940079</v>
       </c>
       <c r="U45" t="s">
@@ -9208,39 +9273,39 @@
         <v>0.84522831540160603</v>
       </c>
       <c r="K46" s="1">
-        <f>(F46/$F$2)/(C46/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.37816089861457514</v>
       </c>
       <c r="M46">
-        <f>(D46-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>2.5420382399319785</v>
       </c>
       <c r="N46">
-        <f>(E46-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.56473241178520306</v>
       </c>
       <c r="O46">
-        <f>(F46-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>1.4377641049229801</v>
       </c>
       <c r="P46">
-        <f>(G46-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.60122259714440818</v>
       </c>
       <c r="Q46">
-        <f>(H46-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>1.2270923779393317</v>
       </c>
       <c r="R46">
-        <f>(I46-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.78102186713194155</v>
       </c>
       <c r="S46">
-        <f>(J46-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.20302894275603459</v>
       </c>
       <c r="T46">
-        <f>ABS(M46)+ABS(N46)+ABS(O46)+ABS(P46)+ABS(Q46)+ABS(R46)+ABS(S46)</f>
+        <f t="shared" si="20"/>
         <v>7.3569005416118776</v>
       </c>
       <c r="U46" t="s">
@@ -9282,39 +9347,39 @@
         <v>0.40635976702000287</v>
       </c>
       <c r="K47" s="1">
-        <f>(F47/$F$2)/(C47/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.36780649305727126</v>
       </c>
       <c r="M47">
-        <f>(D47-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.40879544430802994</v>
       </c>
       <c r="N47">
-        <f>(E47-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.52785113126433114</v>
       </c>
       <c r="O47">
-        <f>(F47-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.53744603857378204</v>
       </c>
       <c r="P47">
-        <f>(G47-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.607740756431983</v>
       </c>
       <c r="Q47">
-        <f>(H47-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.32050057633884094</v>
       </c>
       <c r="R47">
-        <f>(I47-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.42446840604996833</v>
       </c>
       <c r="S47">
-        <f>(J47-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.77873513615956169</v>
       </c>
       <c r="T47">
-        <f>ABS(M47)+ABS(N47)+ABS(O47)+ABS(P47)+ABS(Q47)+ABS(R47)+ABS(S47)</f>
+        <f t="shared" si="20"/>
         <v>3.6055374891264971</v>
       </c>
       <c r="U47" t="s">
@@ -9356,39 +9421,39 @@
         <v>0.43345041815466973</v>
       </c>
       <c r="K48" s="1">
-        <f>(F48/$F$2)/(C48/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.35029189814978218</v>
       </c>
       <c r="M48">
-        <f>(D48-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.42277811285917144</v>
       </c>
       <c r="N48">
-        <f>(E48-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.71533097391209677</v>
       </c>
       <c r="O48">
-        <f>(F48-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.49243595051317751</v>
       </c>
       <c r="P48">
-        <f>(G48-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.61425891571955793</v>
       </c>
       <c r="Q48">
-        <f>(H48-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.27043139252395887</v>
       </c>
       <c r="R48">
-        <f>(I48-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.49577909826636307</v>
       </c>
       <c r="S48">
-        <f>(J48-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.74319771681366487</v>
       </c>
       <c r="T48">
-        <f>ABS(M48)+ABS(N48)+ABS(O48)+ABS(P48)+ABS(Q48)+ABS(R48)+ABS(S48)</f>
+        <f t="shared" si="20"/>
         <v>3.7542121606079908</v>
       </c>
       <c r="U48" t="s">
@@ -9430,39 +9495,39 @@
         <v>0.43345041815466973</v>
       </c>
       <c r="K49" s="1">
-        <f>(F49/$F$2)/(C49/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.34214557493699654</v>
       </c>
       <c r="M49">
-        <f>(D49-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>1.0696877724942422</v>
       </c>
       <c r="N49">
-        <f>(E49-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.61390745247969902</v>
       </c>
       <c r="O49">
-        <f>(F49-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>0.45800962992935557</v>
       </c>
       <c r="P49">
-        <f>(G49-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.61425891571955793</v>
       </c>
       <c r="Q49">
-        <f>(H49-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>1.4728865530305708</v>
       </c>
       <c r="R49">
-        <f>(I49-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.49577909826636307</v>
       </c>
       <c r="S49">
-        <f>(J49-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.74319771681366487</v>
       </c>
       <c r="T49">
-        <f>ABS(M49)+ABS(N49)+ABS(O49)+ABS(P49)+ABS(Q49)+ABS(R49)+ABS(S49)</f>
+        <f t="shared" si="20"/>
         <v>5.4677271387334532</v>
       </c>
       <c r="U49" t="s">
@@ -9504,39 +9569,39 @@
         <v>0.43345041815466973</v>
       </c>
       <c r="K50" s="1">
-        <f>(F50/$F$2)/(C50/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.34214557493699654</v>
       </c>
       <c r="M50">
-        <f>(D50-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-2.2922854291442266E-2</v>
       </c>
       <c r="N50">
-        <f>(E50-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.6661559332176008</v>
       </c>
       <c r="O50">
-        <f>(F50-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.22028192968161514</v>
       </c>
       <c r="P50">
-        <f>(G50-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.61425891571955793</v>
       </c>
       <c r="Q50">
-        <f>(H50-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>0.248467421557546</v>
       </c>
       <c r="R50">
-        <f>(I50-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.49577909826636307</v>
       </c>
       <c r="S50">
-        <f>(J50-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.74319771681366487</v>
       </c>
       <c r="T50">
-        <f>ABS(M50)+ABS(N50)+ABS(O50)+ABS(P50)+ABS(Q50)+ABS(R50)+ABS(S50)</f>
+        <f t="shared" si="20"/>
         <v>3.0110638695477898</v>
       </c>
       <c r="U50" t="s">
@@ -9578,39 +9643,39 @@
         <v>0.43345041815466973</v>
       </c>
       <c r="K51" s="1">
-        <f>(F51/$F$2)/(C51/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.3421455749369966</v>
       </c>
       <c r="M51">
-        <f>(D51-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.56309541831974874</v>
       </c>
       <c r="N51">
-        <f>(E51-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.22358056696713782</v>
       </c>
       <c r="O51">
-        <f>(F51-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.64735439314037457</v>
       </c>
       <c r="P51">
-        <f>(G51-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.61425891571955793</v>
       </c>
       <c r="Q51">
-        <f>(H51-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.52532905558154019</v>
       </c>
       <c r="R51">
-        <f>(I51-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.49577909826636307</v>
       </c>
       <c r="S51">
-        <f>(J51-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.74319771681366487</v>
       </c>
       <c r="T51">
-        <f>ABS(M51)+ABS(N51)+ABS(O51)+ABS(P51)+ABS(Q51)+ABS(R51)+ABS(S51)</f>
+        <f t="shared" si="20"/>
         <v>3.8125951648083869</v>
       </c>
       <c r="U51" t="s">
@@ -9652,39 +9717,39 @@
         <v>0.48763172042400349</v>
       </c>
       <c r="K52" s="1">
-        <f>(F52/$F$2)/(C52/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.30273174645160722</v>
       </c>
       <c r="M52">
-        <f>(D52-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>0.10880860205878504</v>
       </c>
       <c r="N52">
-        <f>(E52-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.54321833148136123</v>
       </c>
       <c r="O52">
-        <f>(F52-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.29460091229331109</v>
       </c>
       <c r="P52">
-        <f>(G52-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.63381339358228261</v>
       </c>
       <c r="Q52">
-        <f>(H52-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>2.5431966382162365E-2</v>
       </c>
       <c r="R52">
-        <f>(I52-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S52">
-        <f>(J52-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.67212287812187144</v>
       </c>
       <c r="T52">
-        <f>ABS(M52)+ABS(N52)+ABS(O52)+ABS(P52)+ABS(Q52)+ABS(R52)+ABS(S52)</f>
+        <f t="shared" si="20"/>
         <v>2.9163965666189262</v>
       </c>
       <c r="U52" t="s">
@@ -9726,39 +9791,39 @@
         <v>0.44119060419314604</v>
       </c>
       <c r="K53" s="1">
-        <f>(F53/$F$2)/(C53/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.28084449276078466</v>
       </c>
       <c r="M53">
-        <f>(D53-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>0.5677835645006386</v>
       </c>
       <c r="N53">
-        <f>(E53-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.58624649208904511</v>
       </c>
       <c r="O53">
-        <f>(F53-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-5.3849278480775115E-2</v>
       </c>
       <c r="P53">
-        <f>(G53-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.64684971215743237</v>
       </c>
       <c r="Q53">
-        <f>(H53-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>0.4578476447834165</v>
       </c>
       <c r="R53">
-        <f>(I53-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S53">
-        <f>(J53-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.73304416842912301</v>
       </c>
       <c r="T53">
-        <f>ABS(M53)+ABS(N53)+ABS(O53)+ABS(P53)+ABS(Q53)+ABS(R53)+ABS(S53)</f>
+        <f t="shared" si="20"/>
         <v>3.6840213431395834</v>
       </c>
       <c r="U53" t="s">
@@ -9800,39 +9865,39 @@
         <v>0.58515806450880414</v>
       </c>
       <c r="K54" s="1">
-        <f>(F54/$F$2)/(C54/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.25660918120274745</v>
       </c>
       <c r="M54">
-        <f>(D54-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.50716474411518297</v>
       </c>
       <c r="N54">
-        <f>(E54-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.77679977478021667</v>
       </c>
       <c r="O54">
-        <f>(F54-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.5782691416985164</v>
       </c>
       <c r="P54">
-        <f>(G54-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.6533678714450073</v>
       </c>
       <c r="Q54">
-        <f>(H54-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.43429417591811831</v>
       </c>
       <c r="R54">
-        <f>(I54-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.78102186713194155</v>
       </c>
       <c r="S54">
-        <f>(J54-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.54418816847664331</v>
       </c>
       <c r="T54">
-        <f>ABS(M54)+ABS(N54)+ABS(O54)+ABS(P54)+ABS(Q54)+ABS(R54)+ABS(S54)</f>
+        <f t="shared" si="20"/>
         <v>4.2751057435656268</v>
       </c>
       <c r="U54" t="s">
@@ -9874,39 +9939,39 @@
         <v>0.55264928314720396</v>
       </c>
       <c r="K55" s="1">
-        <f>(F55/$F$2)/(C55/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.25222269947278586</v>
       </c>
       <c r="M55">
-        <f>(D55-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.11883905435278096</v>
       </c>
       <c r="N55">
-        <f>(E55-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.59546681221926301</v>
       </c>
       <c r="O55">
-        <f>(F55-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.43172466894305972</v>
       </c>
       <c r="P55">
-        <f>(G55-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.65988603073258212</v>
       </c>
       <c r="Q55">
-        <f>(H55-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.23856918464176124</v>
       </c>
       <c r="R55">
-        <f>(I55-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.78102186713194155</v>
       </c>
       <c r="S55">
-        <f>(J55-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.58683307169171928</v>
       </c>
       <c r="T55">
-        <f>ABS(M55)+ABS(N55)+ABS(O55)+ABS(P55)+ABS(Q55)+ABS(R55)+ABS(S55)</f>
+        <f t="shared" si="20"/>
         <v>3.4123406897131079</v>
       </c>
       <c r="U55" t="s">
@@ -9948,39 +10013,39 @@
         <v>0.39010537633920278</v>
       </c>
       <c r="K56" s="1">
-        <f>(F56/$F$2)/(C56/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.18014482922819136</v>
       </c>
       <c r="M56">
-        <f>(D56-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.33103218236571696</v>
       </c>
       <c r="N56">
-        <f>(E56-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.74606537434615661</v>
       </c>
       <c r="O56">
-        <f>(F56-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.5269785762341066</v>
       </c>
       <c r="P56">
-        <f>(G56-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.69247682717045667</v>
       </c>
       <c r="Q56">
-        <f>(H56-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.27498313650712997</v>
       </c>
       <c r="R56">
-        <f>(I56-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.78102186713194155</v>
       </c>
       <c r="S56">
-        <f>(J56-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.80005758776709979</v>
       </c>
       <c r="T56">
-        <f>ABS(M56)+ABS(N56)+ABS(O56)+ABS(P56)+ABS(Q56)+ABS(R56)+ABS(S56)</f>
+        <f t="shared" si="20"/>
         <v>4.152615551522608</v>
       </c>
       <c r="U56" t="s">
@@ -10022,39 +10087,39 @@
         <v>0.2786466973851448</v>
       </c>
       <c r="K57" s="1">
-        <f>(F57/$F$2)/(C57/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.1710727874684983</v>
       </c>
       <c r="M57">
-        <f>(D57-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.59204199532035739</v>
       </c>
       <c r="N57">
-        <f>(E57-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.83826857564833657</v>
       </c>
       <c r="O57">
-        <f>(F57-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.64735439314037457</v>
       </c>
       <c r="P57">
-        <f>(G57-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.69247682717045667</v>
       </c>
       <c r="Q57">
-        <f>(H57-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.49801859168251367</v>
       </c>
       <c r="R57">
-        <f>(I57-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.63840048269915228</v>
       </c>
       <c r="S57">
-        <f>(J57-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.94626868450450352</v>
       </c>
       <c r="T57">
-        <f>ABS(M57)+ABS(N57)+ABS(O57)+ABS(P57)+ABS(Q57)+ABS(R57)+ABS(S57)</f>
+        <f t="shared" si="20"/>
         <v>4.8528295501656951</v>
       </c>
       <c r="U57" t="s">
@@ -10096,39 +10161,39 @@
         <v>0.11821375040581902</v>
       </c>
       <c r="K58" s="1">
-        <f>(F58/$F$2)/(C58/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.12720797016888333</v>
       </c>
       <c r="M58">
-        <f>(D58-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>0.23391668909531382</v>
       </c>
       <c r="N58">
-        <f>(E58-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.2543149674011978</v>
       </c>
       <c r="O58">
-        <f>(F58-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.55105373961536019</v>
       </c>
       <c r="P58">
-        <f>(G58-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.71854946432075628</v>
       </c>
       <c r="Q58">
-        <f>(H58-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>9.8259870112899841E-2</v>
       </c>
       <c r="R58">
-        <f>(I58-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.35315771383357369</v>
       </c>
       <c r="S58">
-        <f>(J58-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-1.1567240510204633</v>
       </c>
       <c r="T58">
-        <f>ABS(M58)+ABS(N58)+ABS(O58)+ABS(P58)+ABS(Q58)+ABS(R58)+ABS(S58)</f>
+        <f t="shared" si="20"/>
         <v>3.3659764953995648</v>
       </c>
       <c r="U58" t="s">
@@ -10170,39 +10235,39 @@
         <v>7.2241736359111616E-2</v>
       </c>
       <c r="K59" s="1">
-        <f>(F59/$F$2)/(C59/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.12672058330999872</v>
       </c>
       <c r="M59">
-        <f>(D59-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>0.66688879423153591</v>
       </c>
       <c r="N59">
-        <f>(E59-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>0.71996552635850208</v>
       </c>
       <c r="O59">
-        <f>(F59-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.58873660403819184</v>
       </c>
       <c r="P59">
-        <f>(G59-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.71854946432075628</v>
       </c>
       <c r="Q59">
-        <f>(H59-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>0.19839823774266399</v>
       </c>
       <c r="R59">
-        <f>(I59-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>0.14601713168118866</v>
       </c>
       <c r="S59">
-        <f>(J59-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-1.2170299747589548</v>
       </c>
       <c r="T59">
-        <f>ABS(M59)+ABS(N59)+ABS(O59)+ABS(P59)+ABS(Q59)+ABS(R59)+ABS(S59)</f>
+        <f t="shared" si="20"/>
         <v>4.2555857331317934</v>
       </c>
       <c r="U59" t="s">
@@ -10244,39 +10309,39 @@
         <v>1.3003512544640092</v>
       </c>
       <c r="K60" s="1">
-        <f>(F60/$F$2)/(C60/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.11404852497899885</v>
       </c>
       <c r="M60">
-        <f>(D60-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.62932911145673454</v>
       </c>
       <c r="N60">
-        <f>(E60-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-1.053409378686756</v>
       </c>
       <c r="O60">
-        <f>(F60-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.66410233288385534</v>
       </c>
       <c r="P60">
-        <f>(G60-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.71854946432075628</v>
       </c>
       <c r="Q60">
-        <f>(H60-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.56174300744690908</v>
       </c>
       <c r="R60">
-        <f>(I60-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-1.0662646359975201</v>
       </c>
       <c r="S60">
-        <f>(J60-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>0.39399970225503045</v>
       </c>
       <c r="T60">
-        <f>ABS(M60)+ABS(N60)+ABS(O60)+ABS(P60)+ABS(Q60)+ABS(R60)+ABS(S60)</f>
+        <f t="shared" si="20"/>
         <v>5.0873976330475621</v>
       </c>
       <c r="U60" t="s">
@@ -10318,39 +10383,39 @@
         <v>0.32508781361600231</v>
       </c>
       <c r="K61" s="1">
-        <f>(F61/$F$2)/(C61/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0.11404852497899885</v>
       </c>
       <c r="M61">
-        <f>(D61-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.56677506793847021</v>
       </c>
       <c r="N61">
-        <f>(E61-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.67844969339122474</v>
       </c>
       <c r="O61">
-        <f>(F61-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.6557283630121149</v>
       </c>
       <c r="P61">
-        <f>(G61-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.71854946432075628</v>
       </c>
       <c r="Q61">
-        <f>(H61-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.52988079956471135</v>
       </c>
       <c r="R61">
-        <f>(I61-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.85233255934833629</v>
       </c>
       <c r="S61">
-        <f>(J61-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.88534739419725184</v>
       </c>
       <c r="T61">
-        <f>ABS(M61)+ABS(N61)+ABS(O61)+ABS(P61)+ABS(Q61)+ABS(R61)+ABS(S61)</f>
+        <f t="shared" si="20"/>
         <v>4.8870633417728655</v>
       </c>
       <c r="U61" t="s">
@@ -10392,39 +10457,39 @@
         <v>0.32508781361600231</v>
       </c>
       <c r="K62" s="1">
-        <f>(F62/$F$2)/(C62/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>8.9100410139842851E-2</v>
       </c>
       <c r="M62">
-        <f>(D62-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.54960336971777013</v>
       </c>
       <c r="N62">
-        <f>(E62-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.82904825551811856</v>
       </c>
       <c r="O62">
-        <f>(F62-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.64630764690640696</v>
       </c>
       <c r="P62">
-        <f>(G62-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.73158578289590603</v>
       </c>
       <c r="Q62">
-        <f>(H62-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.49801859168251367</v>
       </c>
       <c r="R62">
-        <f>(I62-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.92364325156473082</v>
       </c>
       <c r="S62">
-        <f>(J62-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.88534739419725184</v>
       </c>
       <c r="T62">
-        <f>ABS(M62)+ABS(N62)+ABS(O62)+ABS(P62)+ABS(Q62)+ABS(R62)+ABS(S62)</f>
+        <f t="shared" si="20"/>
         <v>5.0635542924826984</v>
       </c>
       <c r="U62" t="s">
@@ -10466,39 +10531,39 @@
         <v>0.32508781361600231</v>
       </c>
       <c r="K63" s="1">
-        <f>(F63/$F$2)/(C63/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>8.553639373424915E-2</v>
       </c>
       <c r="M63">
-        <f>(D63-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.58419207613375168</v>
       </c>
       <c r="N63">
-        <f>(E63-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-0.7890935349538406</v>
       </c>
       <c r="O63">
-        <f>(F63-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.65991534794798512</v>
       </c>
       <c r="P63">
-        <f>(G63-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.73158578289590603</v>
       </c>
       <c r="Q63">
-        <f>(H63-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.53898428753105354</v>
       </c>
       <c r="R63">
-        <f>(I63-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.92364325156473082</v>
       </c>
       <c r="S63">
-        <f>(J63-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.88534739419725184</v>
       </c>
       <c r="T63">
-        <f>ABS(M63)+ABS(N63)+ABS(O63)+ABS(P63)+ABS(Q63)+ABS(R63)+ABS(S63)</f>
+        <f t="shared" si="20"/>
         <v>5.1127616752245197</v>
       </c>
       <c r="U63" t="s">
@@ -10540,39 +10605,39 @@
         <v>0.32508781361600231</v>
       </c>
       <c r="K64" s="1">
-        <f>(F64/$F$2)/(C64/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>5.7024262489499426E-2</v>
       </c>
       <c r="M64">
-        <f>(D64-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.63202752117713024</v>
       </c>
       <c r="N64">
-        <f>(E64-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-1.087217219164222</v>
       </c>
       <c r="O64">
-        <f>(F64-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.66828931781972545</v>
       </c>
       <c r="P64">
-        <f>(G64-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.74462210147105579</v>
       </c>
       <c r="Q64">
-        <f>(H64-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.55719126346373793</v>
       </c>
       <c r="R64">
-        <f>(I64-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-0.99495394378112556</v>
       </c>
       <c r="S64">
-        <f>(J64-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.88534739419725184</v>
       </c>
       <c r="T64">
-        <f>ABS(M64)+ABS(N64)+ABS(O64)+ABS(P64)+ABS(Q64)+ABS(R64)+ABS(S64)</f>
+        <f t="shared" si="20"/>
         <v>5.5696487610742489</v>
       </c>
       <c r="U64" t="s">
@@ -10614,39 +10679,39 @@
         <v>0.65017562723200462</v>
       </c>
       <c r="K65" s="1">
-        <f>(F65/$F$2)/(C65/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>5.7024262489499426E-2</v>
       </c>
       <c r="M65">
-        <f>(D65-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.63202752117713024</v>
       </c>
       <c r="N65">
-        <f>(E65-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-1.087217219164222</v>
       </c>
       <c r="O65">
-        <f>(F65-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.66828931781972545</v>
       </c>
       <c r="P65">
-        <f>(G65-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.74462210147105579</v>
       </c>
       <c r="Q65">
-        <f>(H65-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.56174300744690908</v>
       </c>
       <c r="R65">
-        <f>(I65-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-1.0662646359975201</v>
       </c>
       <c r="S65">
-        <f>(J65-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-0.45889836204649109</v>
       </c>
       <c r="T65">
-        <f>ABS(M65)+ABS(N65)+ABS(O65)+ABS(P65)+ABS(Q65)+ABS(R65)+ABS(S65)</f>
+        <f t="shared" si="20"/>
         <v>5.219062165123054</v>
       </c>
       <c r="U65" t="s">
@@ -10688,39 +10753,39 @@
         <v>0</v>
       </c>
       <c r="K66" s="1">
-        <f>(F66/$F$2)/(C66/$C$2)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M66">
-        <f>(D66-$M$2)/$M$1</f>
+        <f t="shared" si="13"/>
         <v>-0.63202752117713024</v>
       </c>
       <c r="N66">
-        <f>(E66-$N$2)/$N$1</f>
+        <f t="shared" si="14"/>
         <v>-1.087217219164222</v>
       </c>
       <c r="O66">
-        <f>(F66-$O$2)/$O$1</f>
+        <f t="shared" si="15"/>
         <v>-0.67247630275559567</v>
       </c>
       <c r="P66">
-        <f>(G66-$P$2)/$P$1</f>
+        <f t="shared" si="16"/>
         <v>-0.7706947386213554</v>
       </c>
       <c r="Q66">
-        <f>(H66-$Q$2)/$Q$1</f>
+        <f t="shared" si="17"/>
         <v>-0.56174300744690908</v>
       </c>
       <c r="R66">
-        <f>(I66-$R$2)/$R$1</f>
+        <f t="shared" si="18"/>
         <v>-1.0662646359975201</v>
       </c>
       <c r="S66">
-        <f>(J66-$S$2)/$S$1</f>
+        <f t="shared" si="19"/>
         <v>-1.3117964263480126</v>
       </c>
       <c r="T66">
-        <f>ABS(M66)+ABS(N66)+ABS(O66)+ABS(P66)+ABS(Q66)+ABS(R66)+ABS(S66)</f>
+        <f t="shared" si="20"/>
         <v>6.1022198515107444</v>
       </c>
       <c r="U66" t="s">
@@ -10742,7 +10807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>